<commit_message>
changes to add some other fields of MCPD
</commit_message>
<xml_diff>
--- a/vavilov3/tests/data/excels/accessions.xlsx
+++ b/vavilov3/tests/data/excels/accessions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
   <si>
     <t xml:space="preserve">INSTCODE</t>
   </si>
@@ -175,9 +175,15 @@
     <t xml:space="preserve">cruze_de cosas</t>
   </si>
   <si>
+    <t xml:space="preserve">ecu1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP058:CIAM81001</t>
   </si>
   <si>
+    <t xml:space="preserve">algunlao; otro lado</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
@@ -193,6 +199,9 @@
     <t xml:space="preserve">ESP026</t>
   </si>
   <si>
+    <t xml:space="preserve">ecu2</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP004:BGE005836</t>
   </si>
   <si>
@@ -202,6 +211,9 @@
     <t xml:space="preserve">state:Galicia;province:La Coruña;municipality:Fisterra;site:San Salvador</t>
   </si>
   <si>
+    <t xml:space="preserve">ecu3</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP058:CIAM81002</t>
   </si>
   <si>
@@ -211,6 +223,9 @@
     <t xml:space="preserve">1981----</t>
   </si>
   <si>
+    <t xml:space="preserve">ecu4</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP004:BGE005837</t>
   </si>
   <si>
@@ -229,10 +244,16 @@
     <t xml:space="preserve">-9.291666666666666</t>
   </si>
   <si>
+    <t xml:space="preserve">ecu5</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP058:CIAM81003</t>
   </si>
   <si>
     <t xml:space="preserve">CIAM81003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecu6</t>
   </si>
   <si>
     <t xml:space="preserve">ESP004:BGE005838</t>
@@ -250,6 +271,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -333,11 +355,11 @@
   </sheetPr>
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG2" activeCellId="0" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
@@ -350,29 +372,27 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="62.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,14 +569,26 @@
       <c r="AB2" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AC2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="AE2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,13 +596,13 @@
         <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>81001</v>
@@ -618,7 +650,7 @@
         <v>19811031</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z3" s="0" t="n">
         <v>300</v>
@@ -629,11 +661,17 @@
       <c r="AB3" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AD3" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="AE3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +679,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>37</v>
@@ -677,7 +715,7 @@
         <v>46</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>48</v>
@@ -703,14 +741,20 @@
       <c r="AB4" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AD4" s="0" t="s">
+        <v>63</v>
+      </c>
       <c r="AE4" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,13 +762,13 @@
         <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>81002</v>
@@ -754,7 +798,7 @@
         <v>46</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>48</v>
@@ -769,7 +813,7 @@
         <v>75</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="Z5" s="0" t="n">
         <v>300</v>
@@ -780,11 +824,17 @@
       <c r="AB5" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AD5" s="0" t="s">
+        <v>67</v>
+      </c>
       <c r="AE5" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,7 +842,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>37</v>
@@ -828,13 +878,13 @@
         <v>46</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="T6" s="0" t="n">
         <v>1840</v>
@@ -854,11 +904,17 @@
       <c r="AB6" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AD6" s="0" t="s">
+        <v>74</v>
+      </c>
       <c r="AE6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AH6" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="AH6" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,13 +922,13 @@
         <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>81003</v>
@@ -902,13 +958,13 @@
         <v>46</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="T7" s="0" t="n">
         <v>1840</v>
@@ -928,8 +984,11 @@
       <c r="AB7" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="AD7" s="0" t="s">
+        <v>77</v>
+      </c>
       <c r="AE7" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>